<commit_message>
Added Spectrum-KYP core 2 joy
</commit_message>
<xml_diff>
--- a/Cores/Core_Status.xlsx
+++ b/Cores/Core_Status.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
   <si>
     <t>Core</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>KYP</t>
+  </si>
+  <si>
+    <t>2-SINCLAIR</t>
   </si>
 </sst>
 </file>
@@ -196,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +224,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -409,7 +418,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -450,9 +459,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -463,6 +469,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -773,7 +785,7 @@
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,7 +939,7 @@
       <c r="I7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1097,7 +1109,7 @@
       <c r="B14" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>43</v>
       </c>
       <c r="D14" s="10" t="s">
@@ -1228,7 +1240,7 @@
       <c r="I18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="19">
         <v>2</v>
       </c>
     </row>
@@ -1287,31 +1299,31 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="17" t="s">
+      <c r="E21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="18">
+      <c r="J21" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1324,7 +1336,7 @@
         <v>49</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>27</v>
@@ -1338,8 +1350,8 @@
       <c r="I22" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="14">
-        <v>2</v>
+      <c r="J22" s="18" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>